<commit_message>
Fix Subscriptions Report: remove the country.
</commit_message>
<xml_diff>
--- a/reports/subscriptions_report/templates/xlsx/template.xlsx
+++ b/reports/subscriptions_report/templates/xlsx/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\billing_reports\reports\subscriptions_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\global-connect-reports\reports\subscriptions_report\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E368C0-8F20-477E-A029-BC8BECFC85AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBC4E0C-DE41-4A1F-A610-BA91B8FDF7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$I$1:$AA$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$H$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Exported At</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Tier 1 ID</t>
-  </si>
-  <si>
-    <t>Customer Country</t>
   </si>
   <si>
     <t>Item Name</t>
@@ -456,33 +453,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="25.77734375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="2" width="25.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="33" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="12" width="21.6640625" customWidth="1"/>
-    <col min="13" max="14" width="45.77734375" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="45.77734375" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="45.77734375" customWidth="1"/>
-    <col min="21" max="22" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="45.77734375" customWidth="1"/>
-    <col min="24" max="24" width="18.44140625" customWidth="1"/>
-    <col min="25" max="26" width="21.21875" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="21.21875" customWidth="1"/>
+    <col min="5" max="11" width="21.6328125" customWidth="1"/>
+    <col min="12" max="13" width="45.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="19.36328125" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="45.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="45.81640625" customWidth="1"/>
+    <col min="20" max="21" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="45.81640625" customWidth="1"/>
+    <col min="23" max="23" width="18.453125" customWidth="1"/>
+    <col min="24" max="25" width="21.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -498,11 +495,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
@@ -513,56 +510,53 @@
         <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:AA1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="H1:Z1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>